<commit_message>
Fin du projet : restructuration
</commit_message>
<xml_diff>
--- a/mdpSHA1.xlsx
+++ b/mdpSHA1.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ryan\pweb\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ryan\PhpstormProjects\pweb\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1E7F3E8F-9BC1-4F92-ABDC-31F2192FD1CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8390244A-6DC2-48EC-A143-F9FB7F684067}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5415" yWindow="1905" windowWidth="21600" windowHeight="11295" xr2:uid="{87F426FE-F4A2-46AA-ABE8-FBAF7CB07618}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="63">
   <si>
     <t>georgesCroilon@loccar.com</t>
   </si>
@@ -214,6 +214,15 @@
   </si>
   <si>
     <t>e2509805892ecf78e3870368286e48cc30a68d96</t>
+  </si>
+  <si>
+    <t>ryan@ryanmalonzo.fr</t>
+  </si>
+  <si>
+    <t>Souris1234</t>
+  </si>
+  <si>
+    <t>1f1d381923c82fc4e3df69c498053618eadf7a47</t>
   </si>
 </sst>
 </file>
@@ -577,10 +586,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25607346-8EF2-4AA6-9EFD-4704E9DD91D2}">
-  <dimension ref="A1:C20"/>
+  <dimension ref="A1:C21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -808,6 +817,17 @@
       </c>
       <c r="C20" t="s">
         <v>59</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B21" t="s">
+        <v>61</v>
+      </c>
+      <c r="C21" t="s">
+        <v>62</v>
       </c>
     </row>
   </sheetData>
@@ -832,6 +852,7 @@
     <hyperlink ref="A18" r:id="rId18" xr:uid="{F9969F3A-1E0B-426A-B311-98296E8BAE0E}"/>
     <hyperlink ref="A19" r:id="rId19" xr:uid="{2655F7CD-6B4C-4C37-88F5-1C50BE8FF77C}"/>
     <hyperlink ref="A20" r:id="rId20" xr:uid="{66348B93-D866-4CE5-B3A3-1875067AC5BF}"/>
+    <hyperlink ref="A21" r:id="rId21" xr:uid="{B6587FFB-96C7-4854-95A8-CAD368E6861E}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>